<commit_message>
adicionado mapas estilo flashpoint
</commit_message>
<xml_diff>
--- a/winrate.xlsx
+++ b/winrate.xlsx
@@ -444,7 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Saida (0,2*avg - 10) * 2</t>
+          <t>Saida (0,2*avg - 10) * 3</t>
         </is>
       </c>
     </row>
@@ -456,22 +456,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>47,8</t>
+          <t>50,3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>44,1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>46,90</t>
+          <t>47,20</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-1,24</t>
+          <t>-1,68</t>
         </is>
       </c>
     </row>
@@ -483,22 +483,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>52,3</t>
+          <t>54</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>52,7</t>
+          <t>54</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>52,50</t>
+          <t>54,00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1,00</t>
+          <t>2,40</t>
         </is>
       </c>
     </row>
@@ -510,22 +510,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>48,3</t>
+          <t>47,1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>50,9</t>
+          <t>48,6</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>49,60</t>
+          <t>47,85</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-0,16</t>
+          <t>-1,29</t>
         </is>
       </c>
     </row>
@@ -537,22 +537,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>50,2</t>
+          <t>48</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>50,3</t>
+          <t>46,8</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>50,25</t>
+          <t>47,40</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0,10</t>
+          <t>-1,56</t>
         </is>
       </c>
     </row>
@@ -564,22 +564,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>49,9</t>
+          <t>50,1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>50,4</t>
+          <t>47,4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>50,15</t>
+          <t>48,75</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>-0,75</t>
         </is>
       </c>
     </row>
@@ -591,22 +591,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>45,2</t>
+          <t>45,1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>45,7</t>
+          <t>48</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>45,45</t>
+          <t>46,55</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-1,82</t>
+          <t>-2,07</t>
         </is>
       </c>
     </row>
@@ -618,22 +618,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>48,1</t>
+          <t>51,8</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>46,7</t>
+          <t>50,6</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>47,40</t>
+          <t>51,20</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-1,04</t>
+          <t>0,72</t>
         </is>
       </c>
     </row>
@@ -645,22 +645,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>47,9</t>
+          <t>48,8</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>48,1</t>
+          <t>54,1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>48,00</t>
+          <t>51,45</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-0,80</t>
+          <t>0,87</t>
         </is>
       </c>
     </row>
@@ -672,22 +672,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>52,2</t>
+          <t>55,9</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>52,6</t>
+          <t>53</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>52,40</t>
+          <t>54,45</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0,96</t>
+          <t>2,67</t>
         </is>
       </c>
     </row>
@@ -699,22 +699,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>46,7</t>
+          <t>49,4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>49,5</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>46,35</t>
+          <t>49,45</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-1,46</t>
+          <t>-0,33</t>
         </is>
       </c>
     </row>
@@ -726,22 +726,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>50,8</t>
+          <t>50,7</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>47,8</t>
+          <t>49,2</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>49,30</t>
+          <t>49,95</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-0,28</t>
+          <t>-0,03</t>
         </is>
       </c>
     </row>
@@ -753,22 +753,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>49,8</t>
+          <t>43,8</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>50,3</t>
+          <t>46,1</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>50,05</t>
+          <t>44,95</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0,02</t>
+          <t>-3,03</t>
         </is>
       </c>
     </row>
@@ -780,22 +780,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>49,1</t>
+          <t>49,4</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>54,3</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>48,55</t>
+          <t>51,85</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>-0,58</t>
+          <t>1,11</t>
         </is>
       </c>
     </row>
@@ -807,22 +807,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>58,4</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>56,8</t>
+          <t>58,7</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>56,40</t>
+          <t>58,55</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2,56</t>
+          <t>5,13</t>
         </is>
       </c>
     </row>
@@ -834,22 +834,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>53,5</t>
+          <t>52,6</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>53,2</t>
+          <t>30,3</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>53,35</t>
+          <t>41,45</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1,34</t>
+          <t>-5,13</t>
         </is>
       </c>
     </row>
@@ -861,22 +861,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>51,5</t>
+          <t>49,9</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>51,5</t>
+          <t>58,1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>51,50</t>
+          <t>54,00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0,60</t>
+          <t>2,40</t>
         </is>
       </c>
     </row>
@@ -888,22 +888,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>50,8</t>
+          <t>53,6</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>49,7</t>
+          <t>55,9</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>50,25</t>
+          <t>54,75</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0,10</t>
+          <t>2,85</t>
         </is>
       </c>
     </row>
@@ -915,22 +915,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>44,7</t>
+          <t>42,8</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>46,3</t>
+          <t>45,3</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>45,50</t>
+          <t>44,05</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>-1,80</t>
+          <t>-3,57</t>
         </is>
       </c>
     </row>
@@ -942,22 +942,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>46,4</t>
+          <t>50,9</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>54,4</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>47,20</t>
+          <t>52,65</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>-1,12</t>
+          <t>1,59</t>
         </is>
       </c>
     </row>
@@ -969,22 +969,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>43,1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>55,4</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>52,00</t>
+          <t>49,25</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0,80</t>
+          <t>-0,45</t>
         </is>
       </c>
     </row>
@@ -996,22 +996,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>50,9</t>
+          <t>54,9</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>48,6</t>
+          <t>62,6</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>49,75</t>
+          <t>58,75</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>-0,10</t>
+          <t>5,25</t>
         </is>
       </c>
     </row>
@@ -1023,22 +1023,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>48,6</t>
+          <t>49,8</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>46,9</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>48,30</t>
+          <t>48,35</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>-0,68</t>
+          <t>-0,99</t>
         </is>
       </c>
     </row>
@@ -1050,22 +1050,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>52,5</t>
+          <t>54,8</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>50,7</t>
+          <t>47,2</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>51,60</t>
+          <t>51,00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0,64</t>
+          <t>0,60</t>
         </is>
       </c>
     </row>
@@ -1077,22 +1077,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>47,7</t>
+          <t>44,6</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>47,1</t>
+          <t>51,2</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>47,40</t>
+          <t>47,90</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>-1,04</t>
+          <t>-1,26</t>
         </is>
       </c>
     </row>
@@ -1104,22 +1104,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>44,6</t>
+          <t>42,2</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>47,1</t>
+          <t>42,3</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>45,85</t>
+          <t>42,25</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>-1,66</t>
+          <t>-4,65</t>
         </is>
       </c>
     </row>
@@ -1131,22 +1131,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>53,1</t>
+          <t>58</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>52,2</t>
+          <t>60,7</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>52,65</t>
+          <t>59,35</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1,06</t>
+          <t>5,61</t>
         </is>
       </c>
     </row>
@@ -1158,22 +1158,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>47,6</t>
+          <t>37,7</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>48,2</t>
+          <t>36,5</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>47,90</t>
+          <t>37,10</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>-0,84</t>
+          <t>-7,74</t>
         </is>
       </c>
     </row>
@@ -1185,22 +1185,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>50,5</t>
+          <t>48,3</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>51,9</t>
+          <t>48,6</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>51,20</t>
+          <t>48,45</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0,48</t>
+          <t>-0,93</t>
         </is>
       </c>
     </row>
@@ -1212,22 +1212,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>50,3</t>
+          <t>40,5</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>50,4</t>
+          <t>44,6</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>50,35</t>
+          <t>42,55</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0,14</t>
+          <t>-4,47</t>
         </is>
       </c>
     </row>
@@ -1239,22 +1239,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>46,3</t>
+          <t>42,6</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>48,1</t>
+          <t>50,2</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>47,20</t>
+          <t>46,40</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>-1,12</t>
+          <t>-2,16</t>
         </is>
       </c>
     </row>
@@ -1266,22 +1266,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>55,6</t>
+          <t>53,1</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>55,9</t>
+          <t>52,7</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>55,75</t>
+          <t>52,90</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2,30</t>
+          <t>1,74</t>
         </is>
       </c>
     </row>
@@ -1293,22 +1293,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>47,5</t>
+          <t>47,4</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>48,8</t>
+          <t>35,6</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>48,15</t>
+          <t>41,50</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>-0,74</t>
+          <t>-5,10</t>
         </is>
       </c>
     </row>
@@ -1320,22 +1320,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>50,9</t>
+          <t>53,4</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>51,2</t>
+          <t>50,3</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>51,05</t>
+          <t>51,85</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0,42</t>
+          <t>1,11</t>
         </is>
       </c>
     </row>
@@ -1347,22 +1347,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>48,4</t>
+          <t>47,7</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>55,2</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>48,70</t>
+          <t>51,45</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>-0,52</t>
+          <t>0,87</t>
         </is>
       </c>
     </row>
@@ -1374,22 +1374,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>52,2</t>
+          <t>53,1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>54,5</t>
+          <t>41,4</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>53,35</t>
+          <t>47,25</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1,34</t>
+          <t>-1,65</t>
         </is>
       </c>
     </row>
@@ -1401,22 +1401,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>50,4</t>
+          <t>44,8</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>48,6</t>
+          <t>51,7</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>49,50</t>
+          <t>48,25</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>-0,20</t>
+          <t>-1,05</t>
         </is>
       </c>
     </row>
@@ -1428,22 +1428,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>48,2</t>
+          <t>48,8</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>48,9</t>
+          <t>49,1</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>48,55</t>
+          <t>48,95</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>-0,58</t>
+          <t>-0,63</t>
         </is>
       </c>
     </row>
@@ -1455,22 +1455,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>55,3</t>
+          <t>58,9</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>54,4</t>
+          <t>55,5</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>54,85</t>
+          <t>57,20</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1,94</t>
+          <t>4,32</t>
         </is>
       </c>
     </row>
@@ -1482,22 +1482,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>50,9</t>
+          <t>46,6</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>50,6</t>
+          <t>69,6</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>50,75</t>
+          <t>58,10</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0,30</t>
+          <t>4,86</t>
         </is>
       </c>
     </row>
@@ -1509,22 +1509,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>48,7</t>
+          <t>45,9</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>46,8</t>
+          <t>44,4</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>47,75</t>
+          <t>45,15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>-0,90</t>
+          <t>-2,91</t>
         </is>
       </c>
     </row>
@@ -1536,22 +1536,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>48,6</t>
+          <t>54,7</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>54,5</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>48,80</t>
+          <t>54,60</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>-0,48</t>
+          <t>2,76</t>
         </is>
       </c>
     </row>
@@ -1563,22 +1563,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>48,6</t>
+          <t>55,3</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>47,2</t>
+          <t>49,7</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>47,90</t>
+          <t>52,50</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>-0,84</t>
+          <t>1,50</t>
         </is>
       </c>
     </row>
@@ -1590,22 +1590,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>53,1</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>50,3</t>
+          <t>53,4</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>51,15</t>
+          <t>53,25</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0,46</t>
+          <t>1,95</t>
         </is>
       </c>
     </row>
@@ -1617,22 +1617,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>50,8</t>
+          <t>47,9</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>51,8</t>
+          <t>30,5</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>51,30</t>
+          <t>39,20</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0,52</t>
+          <t>-6,48</t>
         </is>
       </c>
     </row>
@@ -1644,22 +1644,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>52,7</t>
+          <t>51,1</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>51,1</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>51,35</t>
+          <t>51,10</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0,54</t>
+          <t>0,66</t>
         </is>
       </c>
     </row>

</xml_diff>